<commit_message>
Checa contas não pagas via planilha excel
</commit_message>
<xml_diff>
--- a/Dados/Contas a Receber.xlsx
+++ b/Dados/Contas a Receber.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documentos\DC Consultoria\02.Hashtag\Conteúdo Youtube\Cobranças automáticas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Desktop\projetos\Automacao-Cobranca\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB983537-828A-4058-9700-8634327237CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67E7B3E-F69B-4759-BB13-5A425476B000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2220" windowWidth="20730" windowHeight="11760" xr2:uid="{308E15D5-FE76-45DA-835A-CDEFE906B9E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{308E15D5-FE76-45DA-835A-CDEFE906B9E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -736,9 +736,9 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -746,7 +746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -757,6 +757,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
@@ -1120,7 +1123,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1131,7 +1134,7 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1174,7 @@
         <v>1195</v>
       </c>
       <c r="C2" s="6">
-        <v>44584</v>
+        <v>44927</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1191,7 +1194,7 @@
         <v>1670</v>
       </c>
       <c r="C3" s="6">
-        <v>44587</v>
+        <v>44954</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1210,8 +1213,8 @@
       <c r="B4" s="4">
         <v>1345</v>
       </c>
-      <c r="C4" s="6">
-        <v>44573</v>
+      <c r="C4" s="10">
+        <v>44954</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1230,8 +1233,8 @@
       <c r="B5" s="4">
         <v>1372</v>
       </c>
-      <c r="C5" s="6">
-        <v>44585</v>
+      <c r="C5" s="10">
+        <v>44954</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -5170,8 +5173,9 @@
     <hyperlink ref="E4" r:id="rId3" xr:uid="{7440A571-9808-4CE4-A9BD-8A37BB1DC37A}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>